<commit_message>
Verify primary inductance value using MAXWELL
The simulated ETD44 with 1mm airgap with 59 turns gave an inductance value of 960uH. This is higher than what is designed for (900uH) but is alright since this inductance value would still ensure CCM operation. I also ran a 2mm air gap with ETD44 and saw the the inductabnce/turn^2 "AL" is expect. Also re organised the folder to separature PLECS model and MAXWELL models.
</commit_message>
<xml_diff>
--- a/24V_150W_100kHz_CCM/24V_150W_100kHz_CCM_Parameter_Calculator.xlsx
+++ b/24V_150W_100kHz_CCM/24V_150W_100kHz_CCM_Parameter_Calculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\150W-12V-Flyback-Converter-in-DCM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\150W-12V-Flyback-Converter-in-DCM\24V_150W_100kHz_CCM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2480D742-2092-43D6-A59A-0C80AF380A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8442B3-D290-483C-A594-F08CAFCE3C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="100kHz" sheetId="1" r:id="rId1"/>
@@ -2763,7 +2763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0073AE27-5FFD-4997-A833-CF47191DE33E}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -2869,8 +2869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CCBFF4-720D-4EBA-A894-2A25016A9E9F}">
   <dimension ref="A7:AJ74"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5577,6 +5577,50 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{58195D6E-58EF-430C-BABE-6889B9535670}">
+          <x14:colorSeries rgb="FF0070C0"/>
+          <x14:colorNegative rgb="FF000000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FF000000"/>
+          <x14:colorFirst rgb="FF000000"/>
+          <x14:colorLast rgb="FF000000"/>
+          <x14:colorHigh rgb="FF000000"/>
+          <x14:colorLow rgb="FF000000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A49:A49</xm:f>
+              <xm:sqref>E49</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A50:A50</xm:f>
+              <xm:sqref>E50</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A51:A51</xm:f>
+              <xm:sqref>E51</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A52:A52</xm:f>
+              <xm:sqref>E52</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A53:A53</xm:f>
+              <xm:sqref>E53</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A54:A54</xm:f>
+              <xm:sqref>E54</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A55:A55</xm:f>
+              <xm:sqref>E55</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A56:A56</xm:f>
+              <xm:sqref>E56</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{85896027-3454-42C8-BCD4-E7B98CDAB80D}">
           <x14:colorSeries rgb="FF0070C0"/>
           <x14:colorNegative rgb="FF000000"/>
@@ -5621,50 +5665,6 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{58195D6E-58EF-430C-BABE-6889B9535670}">
-          <x14:colorSeries rgb="FF0070C0"/>
-          <x14:colorNegative rgb="FF000000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FF000000"/>
-          <x14:colorFirst rgb="FF000000"/>
-          <x14:colorLast rgb="FF000000"/>
-          <x14:colorHigh rgb="FF000000"/>
-          <x14:colorLow rgb="FF000000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A49:A49</xm:f>
-              <xm:sqref>E49</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A50:A50</xm:f>
-              <xm:sqref>E50</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A51:A51</xm:f>
-              <xm:sqref>E51</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A52:A52</xm:f>
-              <xm:sqref>E52</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A53:A53</xm:f>
-              <xm:sqref>E53</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A54:A54</xm:f>
-              <xm:sqref>E54</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A55:A55</xm:f>
-              <xm:sqref>E55</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A56:A56</xm:f>
-              <xm:sqref>E56</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Verified the saturation current for 2mm airgap - ETD34 N87
The simulation result for Bsat of 0.3T roughly matches what the manufacturer says the Isat is. However, the inductance value, does not seem to match the "AL" given by the manifacturer vs the simulated "AL". This could be just me mis-interpreting the simulation result or the manifacturer information.
</commit_message>
<xml_diff>
--- a/24V_150W_100kHz_CCM/24V_150W_100kHz_CCM_Parameter_Calculator.xlsx
+++ b/24V_150W_100kHz_CCM/24V_150W_100kHz_CCM_Parameter_Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\150W-12V-Flyback-Converter-in-DCM\24V_150W_100kHz_CCM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8442B3-D290-483C-A594-F08CAFCE3C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2D17FF-7324-4423-9D8B-2A7DE694B7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="100kHz" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="184">
   <si>
     <t>Po_max</t>
   </si>
@@ -583,6 +583,12 @@
   </si>
   <si>
     <t>AC In Irms @ Pmin</t>
+  </si>
+  <si>
+    <t>Ploss = 2.2W</t>
+  </si>
+  <si>
+    <t>3.7W</t>
   </si>
 </sst>
 </file>
@@ -2213,8 +2219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2761,18 +2767,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0073AE27-5FFD-4997-A833-CF47191DE33E}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>176</v>
       </c>
@@ -2780,7 +2787,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>177</v>
       </c>
@@ -2788,7 +2795,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -2796,7 +2803,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>171</v>
       </c>
@@ -2804,15 +2811,21 @@
         <v>2.34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>172</v>
       </c>
       <c r="B7">
         <v>1.24</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>173</v>
       </c>
@@ -2820,7 +2833,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>174</v>
       </c>
@@ -2828,7 +2841,7 @@
         <v>6.79</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>175</v>
       </c>
@@ -2836,7 +2849,7 @@
         <v>6.14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>178</v>
       </c>
@@ -2844,7 +2857,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>180</v>
       </c>
@@ -2852,7 +2865,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>181</v>
       </c>
@@ -2869,8 +2882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CCBFF4-720D-4EBA-A894-2A25016A9E9F}">
   <dimension ref="A7:AJ74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="C52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N66" sqref="N66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4145,7 +4158,7 @@
         <v>40.964455160817366</v>
       </c>
       <c r="V49" s="8">
-        <f t="shared" ref="V49:V56" si="19">($B$29*Q49)/($B$25*F49)</f>
+        <f>($B$29*Q49)/($B$25*F49)</f>
         <v>8.9583333333333339</v>
       </c>
       <c r="W49">
@@ -4202,18 +4215,18 @@
         <v>40</v>
       </c>
       <c r="B50" s="8">
-        <f t="shared" ref="B50" si="20">A50/1000</f>
+        <f t="shared" ref="B50" si="19">A50/1000</f>
         <v>0.04</v>
       </c>
       <c r="C50" s="8">
         <v>5000</v>
       </c>
       <c r="D50" s="8">
-        <f t="shared" ref="D50" si="21">C50/2</f>
+        <f t="shared" ref="D50" si="20">C50/2</f>
         <v>2500</v>
       </c>
       <c r="E50" s="8">
-        <f t="shared" ref="E50:E56" si="22">D50*$B$15</f>
+        <f t="shared" ref="E50:E56" si="21">D50*$B$15</f>
         <v>2.8750000000000001E-2</v>
       </c>
       <c r="F50" s="8">
@@ -4221,7 +4234,7 @@
         <v>162</v>
       </c>
       <c r="G50" s="8">
-        <f t="shared" ref="G50" si="23">ROUNDUP(F50/3.26,0)</f>
+        <f t="shared" ref="G50" si="22">ROUNDUP(F50/3.26,0)</f>
         <v>50</v>
       </c>
       <c r="H50" s="8">
@@ -4253,7 +4266,7 @@
         <v>1.4081375</v>
       </c>
       <c r="O50" s="8">
-        <f t="shared" ref="O50" si="24">N50+M50</f>
+        <f t="shared" ref="O50" si="23">N50+M50</f>
         <v>1.9338958100000001</v>
       </c>
       <c r="P50" s="8">
@@ -4265,7 +4278,7 @@
         <v>4.5804420889339189E-3</v>
       </c>
       <c r="R50" s="8">
-        <f t="shared" ref="R50" si="25">Q50*1000</f>
+        <f t="shared" ref="R50" si="24">Q50*1000</f>
         <v>4.5804420889339186</v>
       </c>
       <c r="S50" s="8">
@@ -4277,11 +4290,11 @@
         <v>153.33333333333331</v>
       </c>
       <c r="U50" s="8">
-        <f t="shared" ref="U50:U56" si="26">(23.5*P50)/SQRT($B$17)</f>
+        <f t="shared" ref="U50:U56" si="25">(23.5*P50)/SQRT($B$17)</f>
         <v>31.237879618904763</v>
       </c>
       <c r="V50" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="V49:V56" si="26">($B$29*Q50)/($B$25*F50)</f>
         <v>6.75</v>
       </c>
       <c r="W50">
@@ -4349,7 +4362,7 @@
         <v>4000</v>
       </c>
       <c r="E51" s="8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="F51" s="8">
@@ -4413,11 +4426,11 @@
         <v>192.44186046511626</v>
       </c>
       <c r="U51" s="8">
+        <f t="shared" si="25"/>
+        <v>25.325383602605065</v>
+      </c>
+      <c r="V51" s="8">
         <f t="shared" si="26"/>
-        <v>25.325383602605065</v>
-      </c>
-      <c r="V51" s="8">
-        <f t="shared" si="19"/>
         <v>5.375</v>
       </c>
       <c r="W51">
@@ -4485,7 +4498,7 @@
         <v>6000</v>
       </c>
       <c r="E52" s="8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="F52" s="8">
@@ -4549,11 +4562,11 @@
         <v>229.99999999999994</v>
       </c>
       <c r="U52" s="8">
+        <f t="shared" si="25"/>
+        <v>21.917240259490416</v>
+      </c>
+      <c r="V52" s="8">
         <f t="shared" si="26"/>
-        <v>21.917240259490416</v>
-      </c>
-      <c r="V52" s="8">
-        <f t="shared" si="19"/>
         <v>4.5000000000000009</v>
       </c>
       <c r="W52">
@@ -4621,7 +4634,7 @@
         <v>8000</v>
       </c>
       <c r="E53" s="8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="F53" s="8">
@@ -4685,11 +4698,11 @@
         <v>267.25806451612897</v>
       </c>
       <c r="U53" s="8">
+        <f t="shared" si="25"/>
+        <v>19.267269957416143</v>
+      </c>
+      <c r="V53" s="8">
         <f t="shared" si="26"/>
-        <v>19.267269957416143</v>
-      </c>
-      <c r="V53" s="8">
-        <f t="shared" si="19"/>
         <v>3.8750000000000004</v>
       </c>
       <c r="W53">
@@ -4757,7 +4770,7 @@
         <v>10000</v>
       </c>
       <c r="E54" s="12">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.115</v>
       </c>
       <c r="F54" s="12">
@@ -4821,11 +4834,11 @@
         <v>306.66666666666663</v>
       </c>
       <c r="U54" s="12">
+        <f t="shared" si="25"/>
+        <v>17.220508274142549</v>
+      </c>
+      <c r="V54" s="12">
         <f t="shared" si="26"/>
-        <v>17.220508274142549</v>
-      </c>
-      <c r="V54" s="12">
-        <f t="shared" si="19"/>
         <v>3.375</v>
       </c>
       <c r="W54">
@@ -4897,7 +4910,7 @@
         <v>14000</v>
       </c>
       <c r="E55" s="8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.161</v>
       </c>
       <c r="F55" s="8">
@@ -4961,11 +4974,11 @@
         <v>345</v>
       </c>
       <c r="U55" s="8">
+        <f t="shared" si="25"/>
+        <v>16.591272198159864</v>
+      </c>
+      <c r="V55" s="8">
         <f t="shared" si="26"/>
-        <v>16.591272198159864</v>
-      </c>
-      <c r="V55" s="8">
-        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="W55">
@@ -5032,7 +5045,7 @@
         <v>175000</v>
       </c>
       <c r="E56" s="8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>2.0125000000000002</v>
       </c>
       <c r="F56" s="8">
@@ -5096,11 +5109,11 @@
         <v>382.30769230769226</v>
       </c>
       <c r="U56" s="8">
+        <f t="shared" si="25"/>
+        <v>44.353815706883331</v>
+      </c>
+      <c r="V56" s="8">
         <f t="shared" si="26"/>
-        <v>44.353815706883331</v>
-      </c>
-      <c r="V56" s="8">
-        <f t="shared" si="19"/>
         <v>2.7083333333333335</v>
       </c>
       <c r="W56">
@@ -5577,6 +5590,50 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{85896027-3454-42C8-BCD4-E7B98CDAB80D}">
+          <x14:colorSeries rgb="FF0070C0"/>
+          <x14:colorNegative rgb="FF000000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FF000000"/>
+          <x14:colorFirst rgb="FF000000"/>
+          <x14:colorLast rgb="FF000000"/>
+          <x14:colorHigh rgb="FF000000"/>
+          <x14:colorLow rgb="FF000000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A36:A36</xm:f>
+              <xm:sqref>E36</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A37:A37</xm:f>
+              <xm:sqref>E37</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A38:A38</xm:f>
+              <xm:sqref>E38</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A39:A39</xm:f>
+              <xm:sqref>E39</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A40:A40</xm:f>
+              <xm:sqref>E40</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A41:A41</xm:f>
+              <xm:sqref>E41</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A42:A42</xm:f>
+              <xm:sqref>E42</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A43:A43</xm:f>
+              <xm:sqref>E43</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{58195D6E-58EF-430C-BABE-6889B9535670}">
           <x14:colorSeries rgb="FF0070C0"/>
           <x14:colorNegative rgb="FF000000"/>
@@ -5621,50 +5678,6 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{85896027-3454-42C8-BCD4-E7B98CDAB80D}">
-          <x14:colorSeries rgb="FF0070C0"/>
-          <x14:colorNegative rgb="FF000000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FF000000"/>
-          <x14:colorFirst rgb="FF000000"/>
-          <x14:colorLast rgb="FF000000"/>
-          <x14:colorHigh rgb="FF000000"/>
-          <x14:colorLow rgb="FF000000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A36:A36</xm:f>
-              <xm:sqref>E36</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A37:A37</xm:f>
-              <xm:sqref>E37</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A38:A38</xm:f>
-              <xm:sqref>E38</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A39:A39</xm:f>
-              <xm:sqref>E39</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A40:A40</xm:f>
-              <xm:sqref>E40</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A41:A41</xm:f>
-              <xm:sqref>E41</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A42:A42</xm:f>
-              <xm:sqref>E42</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A43:A43</xm:f>
-              <xm:sqref>E43</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
@@ -5675,7 +5688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAF048A-3679-49EC-84A3-0B01C90754DF}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finished schematic of "Power section"
Picked, Fuse, NTC and MOV. Designed Bleed resistor, RCD clamp and RC snubber, designed new transformer ETD34. Pick input and output caps. Ready to do the controller section next!
</commit_message>
<xml_diff>
--- a/24V_150W_100kHz_CCM/24V_150W_100kHz_CCM_Parameter_Calculator.xlsx
+++ b/24V_150W_100kHz_CCM/24V_150W_100kHz_CCM_Parameter_Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\150W-24V-Flyback-Converter-in-CCM\24V_150W_100kHz_CCM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F07B1A9-5CCA-4E34-9FBB-E2E20AE4B2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82D7CA2-D575-4138-8661-868406A9679D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8511,6 +8511,50 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{58195D6E-58EF-430C-BABE-6889B9535670}">
+          <x14:colorSeries rgb="FF0070C0"/>
+          <x14:colorNegative rgb="FF000000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FF000000"/>
+          <x14:colorFirst rgb="FF000000"/>
+          <x14:colorLast rgb="FF000000"/>
+          <x14:colorHigh rgb="FF000000"/>
+          <x14:colorLow rgb="FF000000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A49:A49</xm:f>
+              <xm:sqref>E49</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A50:A50</xm:f>
+              <xm:sqref>E50</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A51:A51</xm:f>
+              <xm:sqref>E51</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A52:A52</xm:f>
+              <xm:sqref>E52</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A53:A53</xm:f>
+              <xm:sqref>E53</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A54:A54</xm:f>
+              <xm:sqref>E54</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A55:A55</xm:f>
+              <xm:sqref>E55</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'core and copper loss - N27'!A56:A56</xm:f>
+              <xm:sqref>E56</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{85896027-3454-42C8-BCD4-E7B98CDAB80D}">
           <x14:colorSeries rgb="FF0070C0"/>
           <x14:colorNegative rgb="FF000000"/>
@@ -8555,50 +8599,6 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{58195D6E-58EF-430C-BABE-6889B9535670}">
-          <x14:colorSeries rgb="FF0070C0"/>
-          <x14:colorNegative rgb="FF000000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FF000000"/>
-          <x14:colorFirst rgb="FF000000"/>
-          <x14:colorLast rgb="FF000000"/>
-          <x14:colorHigh rgb="FF000000"/>
-          <x14:colorLow rgb="FF000000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A49:A49</xm:f>
-              <xm:sqref>E49</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A50:A50</xm:f>
-              <xm:sqref>E50</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A51:A51</xm:f>
-              <xm:sqref>E51</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A52:A52</xm:f>
-              <xm:sqref>E52</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A53:A53</xm:f>
-              <xm:sqref>E53</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A54:A54</xm:f>
-              <xm:sqref>E54</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A55:A55</xm:f>
-              <xm:sqref>E55</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'core and copper loss - N27'!A56:A56</xm:f>
-              <xm:sqref>E56</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
@@ -8640,8 +8640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC23FCA-E224-45E5-80F2-8CA49C5C45B4}">
   <dimension ref="A1:J200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G193" sqref="G193"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>